<commit_message>
update output address format
</commit_message>
<xml_diff>
--- a/DB_Links/MassGIS_Parcel_Download_Links.xlsx
+++ b/DB_Links/MassGIS_Parcel_Download_Links.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="435" yWindow="4125" windowWidth="28365" windowHeight="13500" tabRatio="384"/>
+    <workbookView xWindow="435" yWindow="4125" windowWidth="24240" windowHeight="13500" tabRatio="384"/>
   </bookViews>
   <sheets>
     <sheet name="MassGIS_Parcel_Download_Links" sheetId="1" r:id="rId1"/>
@@ -3596,8 +3596,8 @@
   <dimension ref="A1:F352"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A251" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F271" sqref="F271"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3770,7 +3770,7 @@
         <v>678</v>
       </c>
       <c r="E9" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F9" s="3"/>
     </row>
@@ -3826,7 +3826,7 @@
         <v>92</v>
       </c>
       <c r="E12" s="2">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="F12" s="3"/>
     </row>
@@ -3916,7 +3916,7 @@
         <v>910</v>
       </c>
       <c r="E17" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F17" s="3"/>
     </row>
@@ -4026,7 +4026,7 @@
         <v>212</v>
       </c>
       <c r="E23" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F23" s="3"/>
     </row>
@@ -4044,7 +4044,7 @@
         <v>581</v>
       </c>
       <c r="E24" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F24" s="3"/>
     </row>
@@ -4206,7 +4206,7 @@
         <v>239</v>
       </c>
       <c r="E33" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F33" s="3"/>
     </row>
@@ -4402,7 +4402,7 @@
         <v>299</v>
       </c>
       <c r="E44" s="2">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="F44" s="3"/>
     </row>
@@ -4750,7 +4750,7 @@
         <v>374</v>
       </c>
       <c r="E63" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F63" s="3"/>
     </row>
@@ -4768,7 +4768,7 @@
         <v>515</v>
       </c>
       <c r="E64" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F64" s="3"/>
     </row>
@@ -4840,7 +4840,7 @@
         <v>563</v>
       </c>
       <c r="E68" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F68" s="3"/>
     </row>
@@ -4912,7 +4912,7 @@
         <v>663</v>
       </c>
       <c r="E72" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F72" s="3"/>
     </row>
@@ -4966,7 +4966,7 @@
         <v>609</v>
       </c>
       <c r="E75" s="2">
-        <v>2015</v>
+        <v>2020</v>
       </c>
       <c r="F75" s="3"/>
     </row>
@@ -5112,7 +5112,7 @@
         <v>308</v>
       </c>
       <c r="E83" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F83" s="3"/>
     </row>
@@ -5148,7 +5148,7 @@
         <v>32</v>
       </c>
       <c r="E85" s="2">
-        <v>2014</v>
+        <v>2020</v>
       </c>
       <c r="F85" s="3"/>
     </row>
@@ -5294,7 +5294,7 @@
         <v>146</v>
       </c>
       <c r="E93" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F93" s="3"/>
     </row>
@@ -5476,7 +5476,7 @@
         <v>560</v>
       </c>
       <c r="E103" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F103" s="3"/>
     </row>
@@ -5494,7 +5494,7 @@
         <v>792</v>
       </c>
       <c r="E104" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F104" s="3"/>
     </row>
@@ -5512,7 +5512,7 @@
         <v>305</v>
       </c>
       <c r="E105" s="2">
-        <v>2017</v>
+        <v>2020</v>
       </c>
       <c r="F105" s="3"/>
     </row>
@@ -5800,7 +5800,7 @@
         <v>413</v>
       </c>
       <c r="E121" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F121" s="3"/>
     </row>
@@ -5854,7 +5854,7 @@
         <v>83</v>
       </c>
       <c r="E124" s="2">
-        <v>2013</v>
+        <v>2020</v>
       </c>
       <c r="F124" s="3"/>
     </row>
@@ -5908,7 +5908,7 @@
         <v>29</v>
       </c>
       <c r="E127" s="2">
-        <v>2012</v>
+        <v>2020</v>
       </c>
       <c r="F127" s="3"/>
     </row>
@@ -5982,7 +5982,7 @@
         <v>612</v>
       </c>
       <c r="E131" s="2">
-        <v>2010</v>
+        <v>2020</v>
       </c>
       <c r="F131" s="3"/>
     </row>
@@ -6072,7 +6072,7 @@
         <v>768</v>
       </c>
       <c r="E136" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F136" s="3"/>
     </row>
@@ -6090,7 +6090,7 @@
         <v>840</v>
       </c>
       <c r="E137" s="2">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="F137" s="3"/>
     </row>
@@ -6436,7 +6436,7 @@
         <v>131</v>
       </c>
       <c r="E156" s="2">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="F156" s="3"/>
     </row>
@@ -6526,7 +6526,7 @@
         <v>482</v>
       </c>
       <c r="E161" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F161" s="3"/>
     </row>
@@ -6854,7 +6854,7 @@
         <v>1043</v>
       </c>
       <c r="E179" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F179" s="3"/>
     </row>
@@ -6872,7 +6872,7 @@
         <v>161</v>
       </c>
       <c r="E180" s="2">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="F180" s="3"/>
     </row>
@@ -7234,7 +7234,7 @@
         <v>1025</v>
       </c>
       <c r="E200" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F200" s="3"/>
     </row>
@@ -7252,7 +7252,7 @@
         <v>554</v>
       </c>
       <c r="E201" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F201" s="3"/>
     </row>
@@ -7360,7 +7360,7 @@
         <v>702</v>
       </c>
       <c r="E207" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F207" s="3"/>
     </row>
@@ -7468,7 +7468,7 @@
         <v>783</v>
       </c>
       <c r="E213" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F213" s="3"/>
     </row>
@@ -7486,7 +7486,7 @@
         <v>503</v>
       </c>
       <c r="E214" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F214" s="3"/>
     </row>
@@ -7522,7 +7522,7 @@
         <v>149</v>
       </c>
       <c r="E216" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F216" s="3"/>
     </row>
@@ -7594,7 +7594,7 @@
         <v>729</v>
       </c>
       <c r="E220" s="2">
-        <v>2011</v>
+        <v>2019</v>
       </c>
       <c r="F220" s="3"/>
     </row>
@@ -7864,7 +7864,7 @@
         <v>536</v>
       </c>
       <c r="E235" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F235" s="3"/>
     </row>
@@ -7900,7 +7900,7 @@
         <v>275</v>
       </c>
       <c r="E237" s="2">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="F237" s="3"/>
     </row>
@@ -7954,7 +7954,7 @@
         <v>786</v>
       </c>
       <c r="E240" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F240" s="3"/>
     </row>
@@ -8025,7 +8025,7 @@
         <v>266</v>
       </c>
       <c r="E244" s="2">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="F244" s="3"/>
     </row>
@@ -8135,7 +8135,7 @@
         <v>389</v>
       </c>
       <c r="E250" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F250" s="3"/>
     </row>
@@ -8225,7 +8225,7 @@
         <v>230</v>
       </c>
       <c r="E255" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F255" s="3"/>
     </row>
@@ -8279,7 +8279,7 @@
         <v>627</v>
       </c>
       <c r="E258" s="2">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="F258" s="3"/>
     </row>
@@ -8405,7 +8405,7 @@
         <v>944</v>
       </c>
       <c r="E265" s="2">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="F265" s="3" t="s">
         <v>932</v>
@@ -8443,7 +8443,7 @@
         <v>864</v>
       </c>
       <c r="E267" s="2">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="F267" s="3"/>
     </row>
@@ -8461,7 +8461,7 @@
         <v>566</v>
       </c>
       <c r="E268" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F268" s="3"/>
     </row>
@@ -8569,7 +8569,7 @@
         <v>843</v>
       </c>
       <c r="E274" s="2">
-        <v>2012</v>
+        <v>2020</v>
       </c>
       <c r="F274" s="3"/>
     </row>
@@ -8677,7 +8677,7 @@
         <v>98</v>
       </c>
       <c r="E280" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F280" s="3"/>
     </row>
@@ -8825,7 +8825,7 @@
         <v>386</v>
       </c>
       <c r="E288" s="2">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="F288" s="3"/>
     </row>
@@ -8953,7 +8953,7 @@
         <v>801</v>
       </c>
       <c r="E295" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F295" s="3"/>
     </row>
@@ -8989,7 +8989,7 @@
         <v>422</v>
       </c>
       <c r="E297" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F297" s="3"/>
     </row>
@@ -9079,7 +9079,7 @@
         <v>137</v>
       </c>
       <c r="E302" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F302" s="3"/>
     </row>
@@ -9205,7 +9205,7 @@
         <v>431</v>
       </c>
       <c r="E309" s="2">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="F309" s="3"/>
     </row>
@@ -9313,7 +9313,7 @@
         <v>509</v>
       </c>
       <c r="E315" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F315" s="3"/>
     </row>
@@ -9331,7 +9331,7 @@
         <v>925</v>
       </c>
       <c r="E316" s="2">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="F316" s="3"/>
     </row>
@@ -9367,7 +9367,7 @@
         <v>804</v>
       </c>
       <c r="E318" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F318" s="3"/>
     </row>
@@ -9403,7 +9403,7 @@
         <v>506</v>
       </c>
       <c r="E320" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F320" s="3"/>
     </row>
@@ -9655,7 +9655,7 @@
         <v>116</v>
       </c>
       <c r="E334" s="2">
-        <v>2011</v>
+        <v>2020</v>
       </c>
       <c r="F334" s="3"/>
     </row>
@@ -9709,7 +9709,7 @@
         <v>53</v>
       </c>
       <c r="E337" s="2">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="F337" s="3"/>
     </row>
@@ -9763,7 +9763,7 @@
         <v>834</v>
       </c>
       <c r="E340" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F340" s="3"/>
     </row>
@@ -9799,7 +9799,7 @@
         <v>365</v>
       </c>
       <c r="E342" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F342" s="3"/>
     </row>
@@ -9871,7 +9871,7 @@
         <v>666</v>
       </c>
       <c r="E346" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F346" s="3"/>
     </row>

</xml_diff>